<commit_message>
update report almost done
</commit_message>
<xml_diff>
--- a/BSB2101_U202115666_刘文博/BSB2021_U202115666_刘文博_LOGISIM_FPG/RISC-V单周期硬布线控制器表达式自动生成（2022-8-19）.xlsx
+++ b/BSB2101_U202115666_刘文博/BSB2021_U202115666_刘文博_LOGISIM_FPG/RISC-V单周期硬布线控制器表达式自动生成（2022-8-19）.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_Document\hardware_design\hust-hardware_design\BSB2101_U202115666_刘文博\BSB2021_U202115666_刘文博_LOGISIM_FPG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DCBF8F1-AA54-455C-92E3-734A5E8D1699}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22910596-DCE0-490B-A7F1-74547D2024E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="真值表" sheetId="1" r:id="rId1"/>
@@ -7371,7 +7371,7 @@
   </sheetPr>
   <dimension ref="A1:AX63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="S58" sqref="S58"/>
     </sheetView>
@@ -16686,8 +16686,8 @@
   </sheetPr>
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" customHeight="1"/>

</xml_diff>